<commit_message>
So we made a mistake. For the layout and legend we can only use on character to represent the room, so the rooms like Gr(garage) i had to change the char value. Similarly i had change what they were inside the excel sheet
</commit_message>
<xml_diff>
--- a/MT_ClueLayout.xlsx
+++ b/MT_ClueLayout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameMVTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="24">
   <si>
     <t>P</t>
   </si>
@@ -59,21 +59,6 @@
     <t>LL</t>
   </si>
   <si>
-    <t>Gr</t>
-  </si>
-  <si>
-    <t>GrD</t>
-  </si>
-  <si>
-    <t>Lr</t>
-  </si>
-  <si>
-    <t>LrR</t>
-  </si>
-  <si>
-    <t>LrD</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -83,16 +68,34 @@
     <t>X</t>
   </si>
   <si>
-    <t>Ga</t>
-  </si>
-  <si>
-    <t>GaL</t>
-  </si>
-  <si>
     <t>OU</t>
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>KD</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,19 +572,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
@@ -596,25 +599,25 @@
         <v>4</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>4</v>
@@ -629,22 +632,22 @@
         <v>4</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -652,19 +655,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>4</v>
@@ -679,25 +682,25 @@
         <v>4</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>4</v>
@@ -712,22 +715,22 @@
         <v>4</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -735,52 +738,52 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>4</v>
@@ -795,22 +798,22 @@
         <v>4</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -818,19 +821,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>4</v>
@@ -878,22 +881,22 @@
         <v>4</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="X5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -901,19 +904,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>4</v>
@@ -961,22 +964,22 @@
         <v>4</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -1047,19 +1050,19 @@
         <v>4</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -1130,19 +1133,19 @@
         <v>4</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -1219,13 +1222,13 @@
         <v>4</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -2179,10 +2182,10 @@
         <v>4</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>4</v>
@@ -2259,16 +2262,16 @@
         <v>4</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>4</v>
@@ -2298,13 +2301,13 @@
         <v>4</v>
       </c>
       <c r="Y22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AA22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
@@ -2339,22 +2342,22 @@
         <v>4</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>4</v>
@@ -2375,19 +2378,19 @@
         <v>4</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="X23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Y23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AA23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
@@ -2422,22 +2425,22 @@
         <v>4</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>4</v>
@@ -2458,19 +2461,19 @@
         <v>4</v>
       </c>
       <c r="W24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="X24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Y24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AA24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
@@ -2508,16 +2511,16 @@
         <v>4</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>4</v>
@@ -2538,22 +2541,22 @@
         <v>4</v>
       </c>
       <c r="V25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="X25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Y25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
@@ -2594,10 +2597,10 @@
         <v>4</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>4</v>
@@ -2621,22 +2624,22 @@
         <v>4</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="X26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Y26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AA26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
@@ -2704,22 +2707,22 @@
         <v>4</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W27" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="X27" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Y27" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z27" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AA27" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the string values in DoorDirection. Fixed some errors in the csv and change stuff in her tests
</commit_message>
<xml_diff>
--- a/MT_ClueLayout.xlsx
+++ b/MT_ClueLayout.xlsx
@@ -50,13 +50,7 @@
     <t>GU</t>
   </si>
   <si>
-    <t>BL</t>
-  </si>
-  <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>LL</t>
   </si>
   <si>
     <t>K</t>
@@ -96,6 +90,12 @@
   </si>
   <si>
     <t>KD</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>LR</t>
   </si>
 </sst>
 </file>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,19 +572,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
@@ -599,25 +599,25 @@
         <v>4</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>4</v>
@@ -632,22 +632,22 @@
         <v>4</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -655,19 +655,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>4</v>
@@ -682,25 +682,25 @@
         <v>4</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>4</v>
@@ -715,22 +715,22 @@
         <v>4</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -738,19 +738,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>4</v>
@@ -765,25 +765,25 @@
         <v>4</v>
       </c>
       <c r="K4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>4</v>
@@ -798,22 +798,22 @@
         <v>4</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -821,19 +821,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>4</v>
@@ -881,22 +881,22 @@
         <v>4</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -904,19 +904,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>4</v>
@@ -964,22 +964,22 @@
         <v>4</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -1050,19 +1050,19 @@
         <v>4</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -1133,19 +1133,19 @@
         <v>4</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -1222,13 +1222,13 @@
         <v>4</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -1468,16 +1468,16 @@
         <v>4</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
@@ -1491,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>4</v>
@@ -1548,19 +1548,19 @@
         <v>4</v>
       </c>
       <c r="W13" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y13" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z13" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -1628,22 +1628,22 @@
         <v>4</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
@@ -1711,22 +1711,22 @@
         <v>4</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="W15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -1794,22 +1794,22 @@
         <v>4</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
@@ -1880,19 +1880,19 @@
         <v>4</v>
       </c>
       <c r="W17" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X17" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z17" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA17" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
@@ -1966,16 +1966,16 @@
         <v>4</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Y18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Z18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
@@ -2066,7 +2066,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
@@ -2075,7 +2075,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>4</v>
@@ -2149,7 +2149,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
@@ -2158,7 +2158,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>4</v>
@@ -2182,10 +2182,10 @@
         <v>4</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>4</v>
@@ -2232,16 +2232,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>4</v>
@@ -2262,16 +2262,16 @@
         <v>4</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>4</v>
@@ -2301,13 +2301,13 @@
         <v>4</v>
       </c>
       <c r="Y22" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z22" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA22" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
@@ -2315,16 +2315,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>4</v>
@@ -2342,22 +2342,22 @@
         <v>4</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>4</v>
@@ -2378,19 +2378,19 @@
         <v>4</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="X23" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y23" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z23" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA23" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>4</v>
@@ -2407,7 +2407,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>4</v>
@@ -2425,22 +2425,22 @@
         <v>4</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>4</v>
@@ -2461,19 +2461,19 @@
         <v>4</v>
       </c>
       <c r="W24" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X24" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y24" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA24" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>4</v>
@@ -2490,7 +2490,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>4</v>
@@ -2511,16 +2511,16 @@
         <v>4</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>4</v>
@@ -2541,22 +2541,22 @@
         <v>4</v>
       </c>
       <c r="V25" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X25" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y25" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
@@ -2597,10 +2597,10 @@
         <v>4</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>4</v>
@@ -2624,22 +2624,22 @@
         <v>4</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X26" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y26" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA26" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
@@ -2707,22 +2707,22 @@
         <v>4</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W27" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X27" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y27" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z27" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA27" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I did some stuff with the two step one
</commit_message>
<xml_diff>
--- a/MT_ClueLayout.xlsx
+++ b/MT_ClueLayout.xlsx
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +148,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -176,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,13 +211,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -479,7 +515,7 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,22 +607,22 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -598,25 +634,25 @@
       <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="2" t="s">
@@ -631,22 +667,22 @@
       <c r="U2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA2" s="5" t="s">
+      <c r="V2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -654,19 +690,19 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -681,22 +717,22 @@
       <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -714,22 +750,22 @@
       <c r="U3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA3" s="5" t="s">
+      <c r="V3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -737,19 +773,19 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -764,25 +800,25 @@
       <c r="J4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -797,22 +833,22 @@
       <c r="U4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA4" s="5" t="s">
+      <c r="W4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -820,19 +856,19 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -880,22 +916,22 @@
       <c r="U5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA5" s="5" t="s">
+      <c r="V5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -903,19 +939,19 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -930,7 +966,7 @@
       <c r="J6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -963,22 +999,22 @@
       <c r="U6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA6" s="5" t="s">
+      <c r="V6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1001,7 +1037,7 @@
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -1013,7 +1049,7 @@
       <c r="J7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -1049,19 +1085,19 @@
       <c r="V7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA7" s="5" t="s">
+      <c r="W7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1132,19 +1168,19 @@
       <c r="V8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA8" s="5" t="s">
+      <c r="W8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1194,10 +1230,10 @@
       <c r="O9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="5" t="s">
+      <c r="P9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R9" s="2" t="s">
@@ -1221,13 +1257,13 @@
       <c r="X9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y9" s="5" t="s">
+      <c r="Y9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Z9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA9" s="5" t="s">
+      <c r="AA9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1238,10 +1274,10 @@
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1262,7 +1298,7 @@
       <c r="J10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="L10" s="3" t="s">
@@ -1277,10 +1313,10 @@
       <c r="O10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="5" t="s">
+      <c r="P10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -1318,16 +1354,16 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1336,7 +1372,7 @@
       <c r="G11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1360,10 +1396,10 @@
       <c r="O11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="5" t="s">
+      <c r="P11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R11" s="2" t="s">
@@ -1401,16 +1437,16 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1428,7 +1464,7 @@
       <c r="J12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="10" t="s">
         <v>2</v>
       </c>
       <c r="L12" s="3" t="s">
@@ -1443,10 +1479,10 @@
       <c r="O12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="5" t="s">
+      <c r="P12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -1467,16 +1503,16 @@
       <c r="W12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA12" s="5" t="s">
+      <c r="X12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1484,16 +1520,16 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1526,10 +1562,10 @@
       <c r="O13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="5" t="s">
+      <c r="P13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R13" s="2" t="s">
@@ -1547,19 +1583,19 @@
       <c r="V13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA13" s="5" t="s">
+      <c r="W13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1567,16 +1603,16 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1609,10 +1645,10 @@
       <c r="O14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="5" t="s">
+      <c r="P14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -1627,22 +1663,22 @@
       <c r="U14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="W14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA14" s="5" t="s">
+      <c r="V14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA14" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1650,16 +1686,16 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -1692,10 +1728,10 @@
       <c r="O15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="5" t="s">
+      <c r="P15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1713,19 +1749,19 @@
       <c r="V15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA15" s="5" t="s">
+      <c r="W15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1736,10 +1772,10 @@
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1775,10 +1811,10 @@
       <c r="O16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="5" t="s">
+      <c r="P16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R16" s="2" t="s">
@@ -1793,22 +1829,22 @@
       <c r="U16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="W16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA16" s="5" t="s">
+      <c r="V16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA16" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1858,10 +1894,10 @@
       <c r="O17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q17" s="5" t="s">
+      <c r="P17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R17" s="2" t="s">
@@ -1879,19 +1915,19 @@
       <c r="V17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA17" s="5" t="s">
+      <c r="W17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1929,7 +1965,7 @@
       <c r="K18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M18" s="3" t="s">
@@ -1944,7 +1980,7 @@
       <c r="P18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q18" s="5" t="s">
+      <c r="Q18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="R18" s="2" t="s">
@@ -1965,16 +2001,16 @@
       <c r="W18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="X18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA18" s="5" t="s">
+      <c r="X18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2012,7 +2048,7 @@
       <c r="K19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="9" t="s">
         <v>4</v>
       </c>
       <c r="M19" s="2" t="s">
@@ -2065,7 +2101,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -2074,7 +2110,7 @@
       <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -2148,7 +2184,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -2157,7 +2193,7 @@
       <c r="D21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -2181,10 +2217,10 @@
       <c r="L21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="M21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="O21" s="2" t="s">
@@ -2231,13 +2267,13 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2261,16 +2297,16 @@
       <c r="K22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O22" s="5" t="s">
+      <c r="O22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P22" s="2" t="s">
@@ -2300,13 +2336,13 @@
       <c r="X22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA22" s="5" t="s">
+      <c r="Y22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA22" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2314,16 +2350,16 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
@@ -2341,22 +2377,22 @@
       <c r="J23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O23" s="5" t="s">
+      <c r="O23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P23" s="5" t="s">
+      <c r="P23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="2" t="s">
@@ -2380,16 +2416,16 @@
       <c r="W23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="X23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA23" s="5" t="s">
+      <c r="X23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA23" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2397,7 +2433,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -2406,7 +2442,7 @@
       <c r="D24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -2424,22 +2460,22 @@
       <c r="J24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="M24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O24" s="5" t="s">
+      <c r="O24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P24" s="5" t="s">
+      <c r="P24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q24" s="2" t="s">
@@ -2460,19 +2496,19 @@
       <c r="V24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA24" s="5" t="s">
+      <c r="W24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA24" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2480,7 +2516,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -2489,7 +2525,7 @@
       <c r="D25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -2510,16 +2546,16 @@
       <c r="K25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="5" t="s">
+      <c r="M25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O25" s="5" t="s">
+      <c r="O25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P25" s="2" t="s">
@@ -2540,22 +2576,22 @@
       <c r="U25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="W25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA25" s="5" t="s">
+      <c r="V25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA25" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2596,13 +2632,13 @@
       <c r="L26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="O26" s="9" t="s">
         <v>4</v>
       </c>
       <c r="P26" s="2" t="s">
@@ -2623,22 +2659,22 @@
       <c r="U26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="W26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA26" s="5" t="s">
+      <c r="V26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA26" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2706,22 +2742,22 @@
       <c r="U27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="W27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA27" s="5" t="s">
+      <c r="V27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="W27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="X27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA27" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added room shortcut test
</commit_message>
<xml_diff>
--- a/MT_ClueLayout.xlsx
+++ b/MT_ClueLayout.xlsx
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1227,7 @@
       <c r="N9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P9" s="4" t="s">
@@ -1852,7 +1852,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1935,7 +1935,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2718,7 +2718,7 @@
       <c r="M27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="N27" s="6" t="s">
         <v>4</v>
       </c>
       <c r="O27" s="2" t="s">

</xml_diff>